<commit_message>
2400-Testdaten - new DB Structure + Python Automatic Script for Data
</commit_message>
<xml_diff>
--- a/ReliefGoodsLogistics-LegacyData/ReliefGoodsLogistics-LegacyData.xlsx
+++ b/ReliefGoodsLogistics-LegacyData/ReliefGoodsLogistics-LegacyData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\#_Gso_Klassen-2023\OSP\Hilfgüter-Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Manuela\Desktop\3 Jahr\code-repository-osp-gruppen-fi102-team-hottgenroth-ag\ReliefGoodsLogistics-LegacyData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7A358E4E-738E-4D2C-9E61-AFCAE3FE48CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{948D426C-1AD6-45F0-BFFC-99EFAC3DBAFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1590" windowWidth="28170" windowHeight="15195" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Boxen" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10204" uniqueCount="3718">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10202" uniqueCount="3718">
   <si>
     <t>Guid</t>
   </si>
@@ -10942,9 +10942,6 @@
     <t xml:space="preserve">Latrine kit, raised, </t>
   </si>
   <si>
-    <t>1/3</t>
-  </si>
-  <si>
     <t>Latrine kit, raised, 2/3</t>
   </si>
   <si>
@@ -11179,7 +11176,10 @@
     <t>Training Material</t>
   </si>
   <si>
-    <t>BoxGuid</t>
+    <t>BoxGUID</t>
+  </si>
+  <si>
+    <t>ArticleGUID</t>
   </si>
 </sst>
 </file>
@@ -11532,8 +11532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E3DAEA0-E8FD-4C81-B799-6D305F5C8709}">
   <dimension ref="A1:D144"/>
   <sheetViews>
-    <sheetView topLeftCell="A113" workbookViewId="0">
-      <selection sqref="A1:D144"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A82" sqref="A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -12675,14 +12675,6 @@
         <v>3637</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A82" t="s">
-        <v>3638</v>
-      </c>
-      <c r="B82" t="s">
-        <v>3578</v>
-      </c>
-    </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>1412</v>
@@ -12691,7 +12683,7 @@
         <v>2688</v>
       </c>
       <c r="C83" t="s">
-        <v>3639</v>
+        <v>3638</v>
       </c>
       <c r="D83" t="s">
         <v>3578</v>
@@ -12705,7 +12697,7 @@
         <v>2685</v>
       </c>
       <c r="C84" t="s">
-        <v>3640</v>
+        <v>3639</v>
       </c>
       <c r="D84" t="s">
         <v>3578</v>
@@ -12733,7 +12725,7 @@
         <v>2909</v>
       </c>
       <c r="C86" t="s">
-        <v>3641</v>
+        <v>3640</v>
       </c>
       <c r="D86" t="s">
         <v>3578</v>
@@ -12761,7 +12753,7 @@
         <v>2679</v>
       </c>
       <c r="C88" t="s">
-        <v>3642</v>
+        <v>3641</v>
       </c>
       <c r="D88" t="s">
         <v>3576</v>
@@ -12901,7 +12893,7 @@
         <v>3215</v>
       </c>
       <c r="C98" t="s">
-        <v>3643</v>
+        <v>3642</v>
       </c>
       <c r="D98" t="s">
         <v>3578</v>
@@ -12915,10 +12907,10 @@
         <v>3039</v>
       </c>
       <c r="C99" t="s">
+        <v>3643</v>
+      </c>
+      <c r="D99" t="s">
         <v>3644</v>
-      </c>
-      <c r="D99" t="s">
-        <v>3645</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -12929,7 +12921,7 @@
         <v>3041</v>
       </c>
       <c r="C100" t="s">
-        <v>3646</v>
+        <v>3645</v>
       </c>
       <c r="D100" t="s">
         <v>3613</v>
@@ -12971,7 +12963,7 @@
         <v>3071</v>
       </c>
       <c r="C103" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="D103" t="s">
         <v>3576</v>
@@ -12985,7 +12977,7 @@
         <v>3075</v>
       </c>
       <c r="C104" t="s">
-        <v>3648</v>
+        <v>3647</v>
       </c>
       <c r="D104" t="s">
         <v>3613</v>
@@ -13013,7 +13005,7 @@
         <v>3137</v>
       </c>
       <c r="C106" t="s">
-        <v>3649</v>
+        <v>3648</v>
       </c>
       <c r="D106" t="s">
         <v>3576</v>
@@ -13027,7 +13019,7 @@
         <v>3248</v>
       </c>
       <c r="C107" t="s">
-        <v>3650</v>
+        <v>3649</v>
       </c>
       <c r="D107" t="s">
         <v>3576</v>
@@ -13055,7 +13047,7 @@
         <v>3253</v>
       </c>
       <c r="C109" t="s">
-        <v>3651</v>
+        <v>3650</v>
       </c>
       <c r="D109" t="s">
         <v>3604</v>
@@ -13069,7 +13061,7 @@
         <v>3246</v>
       </c>
       <c r="C110" t="s">
-        <v>3652</v>
+        <v>3651</v>
       </c>
       <c r="D110" t="s">
         <v>3576</v>
@@ -13083,7 +13075,7 @@
         <v>3255</v>
       </c>
       <c r="C111" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="D111" t="s">
         <v>3576</v>
@@ -13094,10 +13086,10 @@
         <v>2027</v>
       </c>
       <c r="B112" s="1" t="s">
+        <v>3653</v>
+      </c>
+      <c r="C112" t="s">
         <v>3654</v>
-      </c>
-      <c r="C112" t="s">
-        <v>3655</v>
       </c>
       <c r="D112" t="s">
         <v>3578</v>
@@ -13108,10 +13100,10 @@
         <v>2031</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>3656</v>
+        <v>3655</v>
       </c>
       <c r="C113" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="D113" t="s">
         <v>3576</v>
@@ -13122,13 +13114,13 @@
         <v>2404</v>
       </c>
       <c r="B114" s="1" t="s">
+        <v>3656</v>
+      </c>
+      <c r="C114" t="s">
         <v>3657</v>
       </c>
-      <c r="C114" t="s">
-        <v>3658</v>
-      </c>
       <c r="D114" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -13136,10 +13128,10 @@
         <v>2038</v>
       </c>
       <c r="B115" s="1" t="s">
+        <v>3658</v>
+      </c>
+      <c r="C115" t="s">
         <v>3659</v>
-      </c>
-      <c r="C115" t="s">
-        <v>3660</v>
       </c>
       <c r="D115" t="s">
         <v>3613</v>
@@ -13150,10 +13142,10 @@
         <v>2099</v>
       </c>
       <c r="B116" s="1" t="s">
+        <v>3660</v>
+      </c>
+      <c r="C116" t="s">
         <v>3661</v>
-      </c>
-      <c r="C116" t="s">
-        <v>3662</v>
       </c>
       <c r="D116" t="s">
         <v>3578</v>
@@ -13164,10 +13156,10 @@
         <v>2129</v>
       </c>
       <c r="B117" s="1" t="s">
+        <v>3662</v>
+      </c>
+      <c r="C117" t="s">
         <v>3663</v>
-      </c>
-      <c r="C117" t="s">
-        <v>3664</v>
       </c>
       <c r="D117" t="s">
         <v>3578</v>
@@ -13178,10 +13170,10 @@
         <v>2133</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>3665</v>
+        <v>3664</v>
       </c>
       <c r="C118" t="s">
-        <v>3647</v>
+        <v>3646</v>
       </c>
       <c r="D118" t="s">
         <v>3576</v>
@@ -13192,10 +13184,10 @@
         <v>2140</v>
       </c>
       <c r="B119" s="1" t="s">
+        <v>3665</v>
+      </c>
+      <c r="C119" t="s">
         <v>3666</v>
-      </c>
-      <c r="C119" t="s">
-        <v>3667</v>
       </c>
       <c r="D119" t="s">
         <v>3613</v>
@@ -13206,10 +13198,10 @@
         <v>2159</v>
       </c>
       <c r="B120" s="1" t="s">
+        <v>3667</v>
+      </c>
+      <c r="C120" t="s">
         <v>3668</v>
-      </c>
-      <c r="C120" t="s">
-        <v>3669</v>
       </c>
       <c r="D120" t="s">
         <v>3613</v>
@@ -13220,10 +13212,10 @@
         <v>2919</v>
       </c>
       <c r="B121" s="1" t="s">
+        <v>3669</v>
+      </c>
+      <c r="C121" t="s">
         <v>3670</v>
-      </c>
-      <c r="C121" t="s">
-        <v>3671</v>
       </c>
       <c r="D121" t="s">
         <v>3578</v>
@@ -13234,13 +13226,13 @@
         <v>2185</v>
       </c>
       <c r="B122" s="1" t="s">
+        <v>3671</v>
+      </c>
+      <c r="C122" t="s">
         <v>3672</v>
       </c>
-      <c r="C122" t="s">
-        <v>3673</v>
-      </c>
       <c r="D122" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -13248,10 +13240,10 @@
         <v>2192</v>
       </c>
       <c r="B123" s="1" t="s">
+        <v>3673</v>
+      </c>
+      <c r="C123" t="s">
         <v>3674</v>
-      </c>
-      <c r="C123" t="s">
-        <v>3675</v>
       </c>
       <c r="D123" t="s">
         <v>3578</v>
@@ -13262,10 +13254,10 @@
         <v>2364</v>
       </c>
       <c r="B124" s="1" t="s">
+        <v>3675</v>
+      </c>
+      <c r="C124" t="s">
         <v>3676</v>
-      </c>
-      <c r="C124" t="s">
-        <v>3677</v>
       </c>
       <c r="D124" t="s">
         <v>3578</v>
@@ -13276,10 +13268,10 @@
         <v>2374</v>
       </c>
       <c r="B125" s="1" t="s">
+        <v>3677</v>
+      </c>
+      <c r="C125" t="s">
         <v>3678</v>
-      </c>
-      <c r="C125" t="s">
-        <v>3679</v>
       </c>
       <c r="D125" t="s">
         <v>3578</v>
@@ -13290,10 +13282,10 @@
         <v>2391</v>
       </c>
       <c r="B126" s="1" t="s">
+        <v>3679</v>
+      </c>
+      <c r="C126" t="s">
         <v>3680</v>
-      </c>
-      <c r="C126" t="s">
-        <v>3681</v>
       </c>
       <c r="D126" t="s">
         <v>3576</v>
@@ -13304,10 +13296,10 @@
         <v>2653</v>
       </c>
       <c r="B127" s="1" t="s">
+        <v>3681</v>
+      </c>
+      <c r="C127" t="s">
         <v>3682</v>
-      </c>
-      <c r="C127" t="s">
-        <v>3683</v>
       </c>
       <c r="D127" t="s">
         <v>3576</v>
@@ -13318,10 +13310,10 @@
         <v>2751</v>
       </c>
       <c r="B128" s="1" t="s">
+        <v>3683</v>
+      </c>
+      <c r="C128" t="s">
         <v>3684</v>
-      </c>
-      <c r="C128" t="s">
-        <v>3685</v>
       </c>
       <c r="D128" t="s">
         <v>3576</v>
@@ -13332,10 +13324,10 @@
         <v>3260</v>
       </c>
       <c r="B129" s="1" t="s">
+        <v>3685</v>
+      </c>
+      <c r="C129" t="s">
         <v>3686</v>
-      </c>
-      <c r="C129" t="s">
-        <v>3687</v>
       </c>
       <c r="D129" t="s">
         <v>3578</v>
@@ -13346,10 +13338,10 @@
         <v>3289</v>
       </c>
       <c r="B130" s="1" t="s">
+        <v>3687</v>
+      </c>
+      <c r="C130" t="s">
         <v>3688</v>
-      </c>
-      <c r="C130" t="s">
-        <v>3689</v>
       </c>
       <c r="D130" t="s">
         <v>3578</v>
@@ -13360,10 +13352,10 @@
         <v>3276</v>
       </c>
       <c r="B131" s="1" t="s">
+        <v>3689</v>
+      </c>
+      <c r="C131" t="s">
         <v>3690</v>
-      </c>
-      <c r="C131" t="s">
-        <v>3691</v>
       </c>
       <c r="D131" t="s">
         <v>3578</v>
@@ -13374,10 +13366,10 @@
         <v>3300</v>
       </c>
       <c r="B132" s="1" t="s">
+        <v>3691</v>
+      </c>
+      <c r="C132" t="s">
         <v>3692</v>
-      </c>
-      <c r="C132" t="s">
-        <v>3693</v>
       </c>
       <c r="D132" t="s">
         <v>3578</v>
@@ -13388,10 +13380,10 @@
         <v>3432</v>
       </c>
       <c r="B133" s="1" t="s">
+        <v>3693</v>
+      </c>
+      <c r="C133" t="s">
         <v>3694</v>
-      </c>
-      <c r="C133" t="s">
-        <v>3695</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
@@ -13399,10 +13391,10 @@
         <v>3442</v>
       </c>
       <c r="B134" s="1" t="s">
+        <v>3695</v>
+      </c>
+      <c r="C134" t="s">
         <v>3696</v>
-      </c>
-      <c r="C134" t="s">
-        <v>3697</v>
       </c>
       <c r="D134" t="s">
         <v>3578</v>
@@ -13413,10 +13405,10 @@
         <v>3466</v>
       </c>
       <c r="B135" s="1" t="s">
+        <v>3697</v>
+      </c>
+      <c r="C135" t="s">
         <v>3698</v>
-      </c>
-      <c r="C135" t="s">
-        <v>3699</v>
       </c>
       <c r="D135" t="s">
         <v>3578</v>
@@ -13427,10 +13419,10 @@
         <v>3469</v>
       </c>
       <c r="B136" s="1" t="s">
+        <v>3699</v>
+      </c>
+      <c r="C136" t="s">
         <v>3700</v>
-      </c>
-      <c r="C136" t="s">
-        <v>3701</v>
       </c>
       <c r="D136" t="s">
         <v>3578</v>
@@ -13441,10 +13433,10 @@
         <v>3472</v>
       </c>
       <c r="B137" s="1" t="s">
+        <v>3701</v>
+      </c>
+      <c r="C137" t="s">
         <v>3702</v>
-      </c>
-      <c r="C137" t="s">
-        <v>3703</v>
       </c>
       <c r="D137" t="s">
         <v>3578</v>
@@ -13455,10 +13447,10 @@
         <v>3475</v>
       </c>
       <c r="B138" s="1" t="s">
+        <v>3703</v>
+      </c>
+      <c r="C138" t="s">
         <v>3704</v>
-      </c>
-      <c r="C138" t="s">
-        <v>3705</v>
       </c>
       <c r="D138" t="s">
         <v>3578</v>
@@ -13469,13 +13461,13 @@
         <v>3478</v>
       </c>
       <c r="B139" s="1" t="s">
+        <v>3705</v>
+      </c>
+      <c r="C139" t="s">
         <v>3706</v>
       </c>
-      <c r="C139" t="s">
+      <c r="D139" t="s">
         <v>3707</v>
-      </c>
-      <c r="D139" t="s">
-        <v>3708</v>
       </c>
     </row>
     <row r="140" spans="1:4" x14ac:dyDescent="0.2">
@@ -13483,13 +13475,13 @@
         <v>3487</v>
       </c>
       <c r="B140" s="1" t="s">
+        <v>3708</v>
+      </c>
+      <c r="C140" t="s">
         <v>3709</v>
       </c>
-      <c r="C140" t="s">
-        <v>3710</v>
-      </c>
       <c r="D140" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="141" spans="1:4" x14ac:dyDescent="0.2">
@@ -13497,13 +13489,13 @@
         <v>3504</v>
       </c>
       <c r="B141" s="1" t="s">
+        <v>3710</v>
+      </c>
+      <c r="C141" t="s">
         <v>3711</v>
       </c>
-      <c r="C141" t="s">
-        <v>3712</v>
-      </c>
       <c r="D141" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="142" spans="1:4" x14ac:dyDescent="0.2">
@@ -13511,13 +13503,13 @@
         <v>3513</v>
       </c>
       <c r="B142" s="1" t="s">
+        <v>3712</v>
+      </c>
+      <c r="C142" t="s">
         <v>3713</v>
       </c>
-      <c r="C142" t="s">
-        <v>3714</v>
-      </c>
       <c r="D142" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.2">
@@ -13525,13 +13517,13 @@
         <v>3522</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>3715</v>
+        <v>3714</v>
       </c>
       <c r="C143" t="s">
-        <v>3712</v>
+        <v>3711</v>
       </c>
       <c r="D143" t="s">
-        <v>3645</v>
+        <v>3644</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.2">
@@ -13542,7 +13534,7 @@
         <v>2659</v>
       </c>
       <c r="C144" t="s">
-        <v>3716</v>
+        <v>3715</v>
       </c>
     </row>
   </sheetData>
@@ -13554,7 +13546,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H1891"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -13570,10 +13564,10 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>3716</v>
+      </c>
+      <c r="B1" t="s">
         <v>3717</v>
-      </c>
-      <c r="B1" t="s">
-        <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>

</xml_diff>